<commit_message>
tc_02 changes pushed work in progress
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>username</t>
   </si>
@@ -58,13 +58,19 @@
   </si>
   <si>
     <t>Add assessment</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +92,12 @@
     </font>
     <font>
       <sz val="7"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -142,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -159,6 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -470,7 +483,7 @@
     <col min="7" max="7" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.2">
+    <row r="1" spans="1:8" ht="28.8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -492,8 +505,11 @@
       <c r="G1" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2">
+    <row r="2" spans="1:8" ht="43.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -514,6 +530,9 @@
       </c>
       <c r="G2" s="7" t="s">
         <v>12</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed till question creation page
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>RMK Nextgen | Add Assessment</t>
+  </si>
+  <si>
+    <t>add assessment 2</t>
   </si>
 </sst>
 </file>
@@ -466,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -483,7 +489,7 @@
     <col min="7" max="7" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8">
+    <row r="1" spans="1:9" ht="28.8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -508,8 +514,11 @@
       <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="43.2">
+    <row r="2" spans="1:9" ht="43.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -529,10 +538,13 @@
         <v>9</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>